<commit_message>
completed to basic mvp
</commit_message>
<xml_diff>
--- a/constants.xlsx
+++ b/constants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kWatts/Repos/ShinyApp_D1toZDN/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kWatts/Repos/ShinyApp_D1toZDN/ZooDietDataConverter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B95F52-A710-A04D-95F5-800EE92B981F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC179488-E62C-A34D-B9E9-5855D0676E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="1220" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - constants" sheetId="1" r:id="rId1"/>
@@ -517,9 +517,6 @@
     <t>Tridecanoic (C13:0)</t>
   </si>
   <si>
-    <t>Units</t>
-  </si>
-  <si>
     <t>%</t>
   </si>
   <si>
@@ -560,6 +557,9 @@
   </si>
   <si>
     <t>na</t>
+  </si>
+  <si>
+    <t>Unit</t>
   </si>
 </sst>
 </file>
@@ -1790,7 +1790,7 @@
   <dimension ref="A1:B168"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1802,26 +1802,26 @@
   <sheetData>
     <row r="1" spans="1:2" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1829,7 +1829,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1837,7 +1837,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1845,7 +1845,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1853,7 +1853,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1861,7 +1861,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1869,7 +1869,7 @@
         <v>26</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1877,7 +1877,7 @@
         <v>14</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1885,7 +1885,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1893,7 +1893,7 @@
         <v>27</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1901,7 +1901,7 @@
         <v>28</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1909,7 +1909,7 @@
         <v>29</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1917,7 +1917,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1925,7 +1925,7 @@
         <v>10</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1933,7 +1933,7 @@
         <v>22</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1941,7 +1941,7 @@
         <v>31</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1949,7 +1949,7 @@
         <v>32</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1957,7 +1957,7 @@
         <v>33</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1965,7 +1965,7 @@
         <v>34</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1973,7 +1973,7 @@
         <v>35</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1981,7 +1981,7 @@
         <v>36</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1989,7 +1989,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1997,7 +1997,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2005,7 +2005,7 @@
         <v>15</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2013,7 +2013,7 @@
         <v>37</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2021,7 +2021,7 @@
         <v>38</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2029,7 +2029,7 @@
         <v>2</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2037,7 +2037,7 @@
         <v>9</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2045,7 +2045,7 @@
         <v>8</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2053,7 +2053,7 @@
         <v>11</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2061,7 +2061,7 @@
         <v>13</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2069,7 +2069,7 @@
         <v>16</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2077,7 +2077,7 @@
         <v>39</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2085,7 +2085,7 @@
         <v>17</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2093,7 +2093,7 @@
         <v>20</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2101,7 +2101,7 @@
         <v>25</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2109,7 +2109,7 @@
         <v>4</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2117,7 +2117,7 @@
         <v>12</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2125,7 +2125,7 @@
         <v>19</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2133,7 +2133,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2141,7 +2141,7 @@
         <v>3</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2149,7 +2149,7 @@
         <v>24</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2157,7 +2157,7 @@
         <v>41</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2165,7 +2165,7 @@
         <v>42</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2173,7 +2173,7 @@
         <v>43</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2181,7 +2181,7 @@
         <v>44</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2189,7 +2189,7 @@
         <v>45</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2197,7 +2197,7 @@
         <v>46</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2205,7 +2205,7 @@
         <v>47</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2213,7 +2213,7 @@
         <v>48</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2221,7 +2221,7 @@
         <v>49</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2229,7 +2229,7 @@
         <v>50</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2237,7 +2237,7 @@
         <v>51</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2245,7 +2245,7 @@
         <v>52</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2253,7 +2253,7 @@
         <v>53</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2261,7 +2261,7 @@
         <v>54</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2269,7 +2269,7 @@
         <v>55</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2277,7 +2277,7 @@
         <v>56</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2285,7 +2285,7 @@
         <v>57</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2293,7 +2293,7 @@
         <v>58</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2301,7 +2301,7 @@
         <v>59</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2309,7 +2309,7 @@
         <v>60</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2317,7 +2317,7 @@
         <v>61</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2325,7 +2325,7 @@
         <v>62</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2333,7 +2333,7 @@
         <v>63</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2341,7 +2341,7 @@
         <v>64</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2349,7 +2349,7 @@
         <v>65</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2357,7 +2357,7 @@
         <v>66</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2365,7 +2365,7 @@
         <v>67</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2373,7 +2373,7 @@
         <v>68</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2381,7 +2381,7 @@
         <v>69</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2389,7 +2389,7 @@
         <v>70</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2397,7 +2397,7 @@
         <v>71</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2405,7 +2405,7 @@
         <v>72</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2413,7 +2413,7 @@
         <v>73</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2421,7 +2421,7 @@
         <v>74</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2429,7 +2429,7 @@
         <v>75</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2437,7 +2437,7 @@
         <v>76</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2445,7 +2445,7 @@
         <v>77</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2453,7 +2453,7 @@
         <v>78</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2461,7 +2461,7 @@
         <v>79</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2469,7 +2469,7 @@
         <v>80</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2477,7 +2477,7 @@
         <v>81</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2485,7 +2485,7 @@
         <v>82</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2493,7 +2493,7 @@
         <v>83</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2501,7 +2501,7 @@
         <v>84</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2509,7 +2509,7 @@
         <v>85</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2517,7 +2517,7 @@
         <v>86</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2525,7 +2525,7 @@
         <v>87</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2533,7 +2533,7 @@
         <v>88</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2541,7 +2541,7 @@
         <v>89</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2549,7 +2549,7 @@
         <v>90</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2557,7 +2557,7 @@
         <v>91</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2565,7 +2565,7 @@
         <v>92</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2573,7 +2573,7 @@
         <v>93</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2581,7 +2581,7 @@
         <v>94</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2589,7 +2589,7 @@
         <v>95</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2597,7 +2597,7 @@
         <v>96</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2605,7 +2605,7 @@
         <v>97</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2613,7 +2613,7 @@
         <v>98</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2621,7 +2621,7 @@
         <v>99</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2629,7 +2629,7 @@
         <v>100</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2637,7 +2637,7 @@
         <v>101</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2645,7 +2645,7 @@
         <v>102</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2653,7 +2653,7 @@
         <v>103</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2661,7 +2661,7 @@
         <v>104</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2669,7 +2669,7 @@
         <v>105</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2677,7 +2677,7 @@
         <v>106</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2685,7 +2685,7 @@
         <v>107</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2693,7 +2693,7 @@
         <v>108</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2701,7 +2701,7 @@
         <v>109</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2709,7 +2709,7 @@
         <v>110</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2717,7 +2717,7 @@
         <v>111</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2725,7 +2725,7 @@
         <v>112</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2733,7 +2733,7 @@
         <v>113</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2741,7 +2741,7 @@
         <v>114</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2749,7 +2749,7 @@
         <v>115</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2757,7 +2757,7 @@
         <v>116</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2765,7 +2765,7 @@
         <v>117</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2773,7 +2773,7 @@
         <v>118</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2781,7 +2781,7 @@
         <v>119</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2789,7 +2789,7 @@
         <v>120</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2797,7 +2797,7 @@
         <v>121</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2805,7 +2805,7 @@
         <v>122</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2813,7 +2813,7 @@
         <v>123</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2821,7 +2821,7 @@
         <v>124</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2829,7 +2829,7 @@
         <v>125</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2837,7 +2837,7 @@
         <v>126</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2845,7 +2845,7 @@
         <v>127</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2853,7 +2853,7 @@
         <v>128</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2861,7 +2861,7 @@
         <v>129</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2869,7 +2869,7 @@
         <v>130</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2877,7 +2877,7 @@
         <v>131</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2885,7 +2885,7 @@
         <v>132</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2893,7 +2893,7 @@
         <v>133</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2901,7 +2901,7 @@
         <v>134</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2909,7 +2909,7 @@
         <v>135</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2917,7 +2917,7 @@
         <v>136</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2925,7 +2925,7 @@
         <v>137</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2933,7 +2933,7 @@
         <v>138</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2941,7 +2941,7 @@
         <v>139</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2949,7 +2949,7 @@
         <v>140</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2957,7 +2957,7 @@
         <v>141</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2965,7 +2965,7 @@
         <v>142</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2973,7 +2973,7 @@
         <v>143</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2981,7 +2981,7 @@
         <v>144</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2989,7 +2989,7 @@
         <v>145</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -2997,7 +2997,7 @@
         <v>146</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3005,7 +3005,7 @@
         <v>147</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3013,7 +3013,7 @@
         <v>148</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3021,7 +3021,7 @@
         <v>149</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3029,7 +3029,7 @@
         <v>150</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3037,7 +3037,7 @@
         <v>151</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3045,7 +3045,7 @@
         <v>152</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3053,7 +3053,7 @@
         <v>153</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3061,7 +3061,7 @@
         <v>154</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3069,7 +3069,7 @@
         <v>155</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3077,7 +3077,7 @@
         <v>156</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3085,7 +3085,7 @@
         <v>157</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3093,7 +3093,7 @@
         <v>158</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3101,7 +3101,7 @@
         <v>159</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3109,7 +3109,7 @@
         <v>160</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3117,7 +3117,7 @@
         <v>161</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3125,7 +3125,7 @@
         <v>162</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3133,7 +3133,7 @@
         <v>163</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3141,7 +3141,7 @@
         <v>164</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>